<commit_message>
updated gant and added project milestones to proposal
</commit_message>
<xml_diff>
--- a/01-planning/GANTT Chart.xlsx
+++ b/01-planning/GANTT Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuahellewell/Desktop/02-msc/01-modules/MSc Project - 771952/01-planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5E35BC-9B0F-AE4E-AFBF-489D9F882448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAC1BFC-D78B-AB4B-A985-7EC8BF21B1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{424283AE-4C7F-2741-A4A2-8357D0D0DADD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>Activity</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>August</t>
+  </si>
+  <si>
+    <t>Week-5</t>
+  </si>
+  <si>
+    <t>Week-6</t>
+  </si>
+  <si>
+    <t>Week-7</t>
+  </si>
+  <si>
+    <t>Week-8</t>
   </si>
   <si>
     <t>Submit Proposal</t>
@@ -169,6 +181,51 @@
   </si>
   <si>
     <t>Ethics approval form</t>
+  </si>
+  <si>
+    <t>Week-9</t>
+  </si>
+  <si>
+    <t>Week-10</t>
+  </si>
+  <si>
+    <t>Week-11</t>
+  </si>
+  <si>
+    <t>Week-12</t>
+  </si>
+  <si>
+    <t>Week-13</t>
+  </si>
+  <si>
+    <t>Week-14</t>
+  </si>
+  <si>
+    <t>Week-15</t>
+  </si>
+  <si>
+    <t>Week-16</t>
+  </si>
+  <si>
+    <t>Week-17</t>
+  </si>
+  <si>
+    <t>Week-18</t>
+  </si>
+  <si>
+    <t>Week-19</t>
+  </si>
+  <si>
+    <t>Week-20</t>
+  </si>
+  <si>
+    <t>Week-21</t>
+  </si>
+  <si>
+    <t>Week-22</t>
+  </si>
+  <si>
+    <t>Week-23</t>
   </si>
 </sst>
 </file>
@@ -230,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -552,24 +609,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -638,7 +682,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1018,14 +1061,15 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D2" sqref="D2:Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="2" width="62.6640625" customWidth="1"/>
-    <col min="3" max="26" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="25" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1075,81 +1119,81 @@
         <v>2</v>
       </c>
       <c r="D2" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="F2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="G2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="45" t="s">
-        <v>2</v>
-      </c>
       <c r="H2" s="45" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="I2" s="45" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J2" s="45" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="K2" s="45" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="L2" s="45" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="M2" s="45" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="N2" s="45" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="O2" s="45" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="P2" s="45" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="Q2" s="45" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="R2" s="45" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="S2" s="45" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="T2" s="45" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="U2" s="45" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="V2" s="45" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="W2" s="45" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="X2" s="45" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="Y2" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z2" s="46" t="s">
-        <v>5</v>
+        <v>61</v>
+      </c>
+      <c r="Z2" s="45" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>11</v>
+      <c r="A3" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>15</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15"/>
@@ -1177,9 +1221,9 @@
       <c r="Z3" s="16"/>
     </row>
     <row r="4" spans="1:26" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="49" t="s">
-        <v>43</v>
+      <c r="A4" s="50"/>
+      <c r="B4" s="48" t="s">
+        <v>47</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="17"/>
@@ -1207,11 +1251,11 @@
       <c r="Z4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="46" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="11"/>
@@ -1239,9 +1283,9 @@
       <c r="Z5" s="13"/>
     </row>
     <row r="6" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="53"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="34" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="21"/>
       <c r="D6" s="1"/>
@@ -1269,9 +1313,9 @@
       <c r="Z6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="53"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="34" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="1"/>
@@ -1299,9 +1343,9 @@
       <c r="Z7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="53"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="35" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="1"/>
@@ -1329,9 +1373,9 @@
       <c r="Z8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="36" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="1"/>
@@ -1359,9 +1403,9 @@
       <c r="Z9" s="4"/>
     </row>
     <row r="10" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="36" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="1"/>
@@ -1388,9 +1432,9 @@
       <c r="Z10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53"/>
+      <c r="A11" s="52"/>
       <c r="B11" s="36" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="1"/>
@@ -1418,9 +1462,9 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="36" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="1"/>
@@ -1448,9 +1492,9 @@
       <c r="Z12" s="4"/>
     </row>
     <row r="13" spans="1:26" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="37" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="24"/>
@@ -1478,11 +1522,11 @@
       <c r="Z13" s="26"/>
     </row>
     <row r="14" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="54" t="s">
-        <v>18</v>
+      <c r="A14" s="53" t="s">
+        <v>22</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="18"/>
@@ -1510,9 +1554,9 @@
       <c r="Z14" s="16"/>
     </row>
     <row r="15" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="55"/>
+      <c r="A15" s="54"/>
       <c r="B15" s="36" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1540,9 +1584,9 @@
       <c r="Z15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="55"/>
+      <c r="A16" s="54"/>
       <c r="B16" s="36" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1570,9 +1614,9 @@
       <c r="Z16" s="4"/>
     </row>
     <row r="17" spans="1:26" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="39" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1600,11 +1644,11 @@
       <c r="Z17" s="6"/>
     </row>
     <row r="18" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="57" t="s">
-        <v>37</v>
+      <c r="A18" s="56" t="s">
+        <v>41</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -1632,9 +1676,9 @@
       <c r="Z18" s="11"/>
     </row>
     <row r="19" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="58"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="36" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1662,9 +1706,9 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="58"/>
+      <c r="A20" s="57"/>
       <c r="B20" s="36" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1692,9 +1736,9 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="58"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="36" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1722,9 +1766,9 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="37" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -1752,11 +1796,11 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="52" t="s">
-        <v>26</v>
+      <c r="A23" s="51" t="s">
+        <v>30</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
@@ -1784,9 +1828,9 @@
       <c r="Z23" s="16"/>
     </row>
     <row r="24" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="53"/>
+      <c r="A24" s="52"/>
       <c r="B24" s="36" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1814,9 +1858,9 @@
       <c r="Z24" s="4"/>
     </row>
     <row r="25" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="53"/>
+      <c r="A25" s="52"/>
       <c r="B25" s="42" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -1844,9 +1888,9 @@
       <c r="Z25" s="10"/>
     </row>
     <row r="26" spans="1:26" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="60"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="41" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
@@ -1874,11 +1918,11 @@
       <c r="Z26" s="26"/>
     </row>
     <row r="27" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="52" t="s">
-        <v>38</v>
+      <c r="A27" s="51" t="s">
+        <v>42</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -1906,9 +1950,9 @@
       <c r="Z27" s="16"/>
     </row>
     <row r="28" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="53"/>
+      <c r="A28" s="52"/>
       <c r="B28" s="36" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1936,9 +1980,9 @@
       <c r="Z28" s="4"/>
     </row>
     <row r="29" spans="1:26" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="60"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="39" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>

</xml_diff>